<commit_message>
Adding papers back to 2011
</commit_message>
<xml_diff>
--- a/conference_papers/ConferenceStats.xlsx
+++ b/conference_papers/ConferenceStats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="2740" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="12700" yWindow="5380" windowWidth="32140" windowHeight="19480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="By Topic" sheetId="1" r:id="rId1"/>
+    <sheet name="By Conf and Year" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Analysis</t>
   </si>
@@ -99,14 +100,37 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Oakland</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>Eurocrypt</t>
+  </si>
+  <si>
+    <t>Asiacrypt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,8 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,6 +842,55 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B2:B12)</f>
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:L13" si="2">SUM(C2:C12)</f>
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
@@ -850,4 +924,318 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>2012</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+      <c r="F1">
+        <v>2016</v>
+      </c>
+      <c r="G1">
+        <v>2017</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <f>SUM(B2:G2)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H11" si="0">SUM(B3:G3)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2:B10)</f>
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:G11" si="1">SUM(C2:C10)</f>
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>